<commit_message>
1. excel reader 03
</commit_message>
<xml_diff>
--- a/zodiac-component-parent/zodiac-component-office/src/test/resources/test.xlsx
+++ b/zodiac-component-parent/zodiac-component-office/src/test/resources/test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangguangyong/IdeaProjects/zodiac-parent/zodiac-component-parent/zodiac-component-office/src/test/resources/"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>姓名</t>
     <rPh sb="0" eb="2">
@@ -130,11 +130,15 @@
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>zhangsan</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="6">
     <font>
       <sz val="12"/>
@@ -540,11 +544,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="20.83203125" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="1" width="22.33203125" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="1" width="17.5" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="1" width="18.33203125" collapsed="false"/>
+    <col min="5" max="16384" style="1" width="10.83203125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -573,6 +577,46 @@
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17">

</xml_diff>